<commit_message>
Se crea Scraping para recoger 100 articulos de MercadoLibre
</commit_message>
<xml_diff>
--- a/Producto.xlsx
+++ b/Producto.xlsx
@@ -19,7 +19,7 @@
     <t>PRODUCTO A BUSCAR</t>
   </si>
   <si>
-    <t>Bicicleta Electrica</t>
+    <t>bicicletas electricas</t>
   </si>
 </sst>
 </file>
@@ -361,10 +361,13 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="19.21875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">

</xml_diff>

<commit_message>
Se realiza DataScraping y ElementExists para confirmar lo Mas Vendido
</commit_message>
<xml_diff>
--- a/Producto.xlsx
+++ b/Producto.xlsx
@@ -14,12 +14,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>PRODUCTO A BUSCAR</t>
   </si>
   <si>
     <t>bicicletas electricas</t>
+  </si>
+  <si>
+    <t>Portatiles</t>
   </si>
 </sst>
 </file>
@@ -358,10 +361,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -379,6 +382,11 @@
         <v>1</v>
       </c>
     </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>